<commit_message>
bess corrected - storage from 20 to 5
</commit_message>
<xml_diff>
--- a/pyecom_tomas/data/EC_V4_new_UC2.xlsx
+++ b/pyecom_tomas/data/EC_V4_new_UC2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\laris\EV4EU2\task2_5\energy_communities_management\pyecom_tomas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C431DFF-6765-46C4-8F65-44695A54D814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD7E7FA-B658-4FD8-AB01-C54D55583D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Information" sheetId="1" r:id="rId1"/>
@@ -7630,9 +7630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD63"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64:AD87"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18535,8 +18535,8 @@
   <dimension ref="A1:AD63"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19567,76 +19567,76 @@
         <v>105</v>
       </c>
       <c r="G19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="K19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="N19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="P19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="R19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="S19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="T19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="U19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="V19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="W19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="X19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Y19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Z19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AA19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AB19" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AC19" s="10">
-        <v>20</v>
-      </c>
-      <c r="AD19" s="20">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="AD19" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
@@ -19659,76 +19659,76 @@
         <v>108</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="K20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="N20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="P20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Q20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="R20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="S20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="T20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="U20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="V20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="W20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="X20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Y20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Z20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AA20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AB20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AC20">
-        <v>20</v>
-      </c>
-      <c r="AD20" s="21">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="AD20">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
@@ -25877,8 +25877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED44E71-8461-49EC-BDE2-25D71C22BD0F}">
   <dimension ref="A1:AD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28458,6 +28458,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D9AF0C12AF32784AA732DC10CF87510A" ma:contentTypeVersion="12" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="704088ab89168f16f5be5ae1239f37bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbae9298-c5c8-4c5d-86f9-781c8fd812a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa1512bd7375e312c8e45d43a3c9a072" ns2:_="">
     <xsd:import namespace="cbae9298-c5c8-4c5d-86f9-781c8fd812a7"/>
@@ -28647,22 +28662,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C9FA379-60F3-40CB-BCC9-DB4DA962BF76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{190C380E-3337-4C81-80E6-9871B5E8C842}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43CD6172-0F07-4FF1-9B13-D3C7D570AF8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28678,21 +28695,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{190C380E-3337-4C81-80E6-9871B5E8C842}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C9FA379-60F3-40CB-BCC9-DB4DA962BF76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>